<commit_message>
add screen control and more display layout
</commit_message>
<xml_diff>
--- a/LightDrumFirmware/Nextion/DisplayColors.xlsx
+++ b/LightDrumFirmware/Nextion/DisplayColors.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -106,10 +106,16 @@
     <t xml:space="preserve">Slider Low</t>
   </si>
   <si>
+    <t xml:space="preserve">Slider Center</t>
+  </si>
+  <si>
     <t xml:space="preserve">Slider High</t>
   </si>
   <si>
-    <t xml:space="preserve">Slider Center</t>
+    <t xml:space="preserve">Slider Center Highlight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F7EA46</t>
   </si>
 </sst>
 </file>
@@ -143,7 +149,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +220,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF231AA3"/>
         <bgColor rgb="FF000080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7EA46"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -251,7 +263,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -260,11 +272,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -309,6 +321,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -328,7 +344,7 @@
       <rgbColor rgb="FFC62306"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFF7EA46"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF690800"/>
@@ -389,10 +405,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -453,6 +469,9 @@
         <v>8</v>
       </c>
       <c r="B3" s="5"/>
+      <c r="C3" s="1" t="n">
+        <v>35206</v>
+      </c>
       <c r="D3" s="1" t="n">
         <v>140</v>
       </c>
@@ -716,6 +735,27 @@
       </c>
       <c r="G15" s="2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="1" t="n">
+        <v>63304</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>247</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix screen ctrl bugs and add I2S data transfer
</commit_message>
<xml_diff>
--- a/LightDrumFirmware/Nextion/DisplayColors.xlsx
+++ b/LightDrumFirmware/Nextion/DisplayColors.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Text</t>
   </si>
   <si>
-    <t xml:space="preserve">FFFFFF</t>
+    <t xml:space="preserve">F5F5F5</t>
   </si>
   <si>
     <t xml:space="preserve">Button Normal</t>
@@ -170,7 +170,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFAFAFA"/>
+        <fgColor rgb="FFF5F5F5"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
@@ -340,7 +340,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFAFAFA"/>
+      <rgbColor rgb="FFF5F5F5"/>
       <rgbColor rgb="FFC62306"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -408,7 +408,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -494,13 +494,13 @@
         <v>63422</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>11</v>

</xml_diff>